<commit_message>
Update the file path
</commit_message>
<xml_diff>
--- a/Testmaven/CaseCreation.xlsx
+++ b/Testmaven/CaseCreation.xlsx
@@ -4,17 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510"/>
+    <workbookView windowWidth="28800" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Variable Value-01</t>
+  </si>
+  <si>
+    <t>Variable Value-02</t>
+  </si>
   <si>
     <t>appURL</t>
   </si>
@@ -31,49 +41,100 @@
     <t>password</t>
   </si>
   <si>
-    <t>caseNumber</t>
+    <t>Case_No</t>
   </si>
   <si>
     <t>P1194US00</t>
   </si>
   <si>
+    <t>TM1193A200</t>
+  </si>
+  <si>
     <t>Case type</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>Country</t>
   </si>
   <si>
     <t>US</t>
   </si>
   <si>
+    <t>In</t>
+  </si>
+  <si>
     <t>Application type</t>
   </si>
   <si>
     <t>With</t>
   </si>
   <si>
+    <t>Di</t>
+  </si>
+  <si>
     <t>Catchword</t>
   </si>
   <si>
     <t>Test Trial</t>
   </si>
   <si>
+    <t>Test Catchword</t>
+  </si>
+  <si>
     <t>Service level</t>
   </si>
   <si>
     <t>Nor</t>
   </si>
   <si>
+    <t>Man</t>
+  </si>
+  <si>
     <t>Team</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>Document path</t>
   </si>
   <si>
     <t>C:\Users\selvamuthukumar.g.ZUCISYSTEMS\OneDrive - zucisystems.com\SG\Patricia\Automation\Testmaven\Test Document.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\selvamuthukumar.g.ZUCISYSTEMS\OneDrive - zucisystems.com\SG\Patricia\Automation\Testmaven\TM1193IN00 Classes.pdf</t>
+  </si>
+  <si>
+    <t>Document type</t>
+  </si>
+  <si>
+    <t>TXT</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Negative case search</t>
+  </si>
+  <si>
+    <t>P00000</t>
+  </si>
+  <si>
+    <t>@0000000</t>
+  </si>
+  <si>
+    <t>CaseNo</t>
+  </si>
+  <si>
+    <t>D1049IN00</t>
+  </si>
+  <si>
+    <t>D1053IN00</t>
   </si>
 </sst>
 </file>
@@ -81,8 +142,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -103,7 +164,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,14 +186,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,7 +200,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,6 +208,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -166,6 +248,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,13 +277,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,45 +286,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -248,6 +309,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -266,169 +369,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,6 +500,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -460,8 +545,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -477,6 +562,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,51 +600,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -560,135 +621,136 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,147 +1070,248 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="30.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="35.1428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5714285714286" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7142857142857" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>4</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>5</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>6</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>7</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>8</v>
       </c>
-      <c r="J1">
+      <c r="J1" s="1">
         <v>9</v>
       </c>
-      <c r="K1">
+      <c r="K1" s="1">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="L1" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C8" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="15.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="18.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>